<commit_message>
AC units method modification
</commit_message>
<xml_diff>
--- a/Test Data/Verify AC Calculation.xlsx
+++ b/Test Data/Verify AC Calculation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Shared\Scripts\work_06_12_2019_latest\consys-uiauto\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -164,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -187,22 +187,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -219,7 +208,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,7 +525,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +534,7 @@
     <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,7 +600,7 @@
       <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -628,7 +617,7 @@
       <c r="D8" s="1">
         <v>250</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -643,6 +632,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -655,6 +645,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -667,6 +658,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -679,6 +671,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>